<commit_message>
Awful class to export to excel... it works but should be refactored and tested
</commit_message>
<xml_diff>
--- a/madetools/core/src/main/resources/ExperimentSummary.xlsx
+++ b/madetools/core/src/main/resources/ExperimentSummary.xlsx
@@ -8,14 +8,15 @@
   </bookViews>
   <sheets>
     <sheet name="Experiment info" sheetId="2" r:id="rId1"/>
-    <sheet name="Data summary" sheetId="1" r:id="rId2"/>
+    <sheet name="Data" sheetId="1" r:id="rId2"/>
+    <sheet name="Summary" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="18">
   <si>
     <t>Iteration</t>
   </si>
@@ -45,13 +46,40 @@
   </si>
   <si>
     <t>Chromosome</t>
+  </si>
+  <si>
+    <t>Started</t>
+  </si>
+  <si>
+    <t>Ended</t>
+  </si>
+  <si>
+    <t>Experiment</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Info</t>
+  </si>
+  <si>
+    <t>Made version</t>
+  </si>
+  <si>
+    <t>Report version</t>
+  </si>
+  <si>
+    <t>1.0</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="d\-m\-yy\ h:mm;@"/>
+  </numFmts>
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -80,6 +108,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -100,7 +136,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -146,72 +182,60 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -510,83 +534,323 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
+  <cols>
+    <col min="1" max="1" width="13.7109375" style="4" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" style="4" customWidth="1"/>
+    <col min="3" max="3" width="12" style="4" customWidth="1"/>
+    <col min="4" max="4" width="13" style="4" customWidth="1"/>
+    <col min="5" max="5" width="14.140625" style="4" customWidth="1"/>
+    <col min="6" max="6" width="13.28515625" style="4" customWidth="1"/>
+    <col min="7" max="16384" width="11.42578125" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:BI2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection sqref="A1:A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" style="2" customWidth="1"/>
-    <col min="2" max="3" width="11.42578125" style="3"/>
-    <col min="4" max="4" width="11.42578125" style="2"/>
-    <col min="5" max="6" width="11.42578125" style="3"/>
-    <col min="7" max="7" width="11.42578125" style="2"/>
-    <col min="8" max="8" width="43.7109375" style="2" customWidth="1"/>
-    <col min="9" max="16384" width="11.42578125" style="3"/>
+    <col min="1" max="1" width="11.42578125" style="8" customWidth="1"/>
+    <col min="2" max="7" width="11.42578125" style="8"/>
+    <col min="8" max="8" width="55.140625" style="8" customWidth="1"/>
+    <col min="9" max="61" width="11.42578125" style="8"/>
+    <col min="62" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="10" customFormat="1">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:61" s="2" customFormat="1">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="8"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="7" t="s">
+      <c r="C1" s="12"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="8"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="4" t="s">
+      <c r="F1" s="12"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="14" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" s="11" customFormat="1" ht="25.5">
-      <c r="A2" s="6"/>
-      <c r="B2" s="11" t="s">
+      <c r="I1" s="11"/>
+      <c r="J1" s="13"/>
+      <c r="K1" s="11"/>
+      <c r="L1" s="13"/>
+      <c r="M1" s="11"/>
+      <c r="N1" s="13"/>
+      <c r="O1" s="11"/>
+      <c r="P1" s="13"/>
+      <c r="Q1" s="11"/>
+      <c r="R1" s="13"/>
+      <c r="S1" s="11"/>
+      <c r="T1" s="13"/>
+      <c r="U1" s="11"/>
+      <c r="V1" s="13"/>
+      <c r="W1" s="11"/>
+      <c r="X1" s="13"/>
+      <c r="Y1" s="11"/>
+      <c r="Z1" s="13"/>
+      <c r="AA1" s="11"/>
+      <c r="AB1" s="13"/>
+      <c r="AC1" s="11"/>
+      <c r="AD1" s="13"/>
+      <c r="AE1" s="11"/>
+      <c r="AF1" s="13"/>
+      <c r="AG1" s="11"/>
+      <c r="AH1" s="13"/>
+      <c r="AI1" s="11"/>
+      <c r="AJ1" s="13"/>
+      <c r="AK1" s="11"/>
+      <c r="AL1" s="13"/>
+      <c r="AM1" s="11"/>
+      <c r="AN1" s="13"/>
+      <c r="AO1" s="11"/>
+      <c r="AP1" s="13"/>
+      <c r="AQ1" s="11"/>
+      <c r="AR1" s="13"/>
+      <c r="AS1" s="11"/>
+      <c r="AT1" s="13"/>
+      <c r="AU1" s="11"/>
+      <c r="AV1" s="13"/>
+      <c r="AW1" s="11"/>
+      <c r="AX1" s="13"/>
+      <c r="AY1" s="11"/>
+      <c r="AZ1" s="13"/>
+      <c r="BA1" s="11"/>
+      <c r="BB1" s="13"/>
+      <c r="BC1" s="11"/>
+      <c r="BD1" s="13"/>
+      <c r="BE1" s="11"/>
+      <c r="BF1" s="13"/>
+      <c r="BG1" s="11"/>
+      <c r="BH1" s="13"/>
+      <c r="BI1" s="6"/>
+    </row>
+    <row r="2" spans="1:61" s="3" customFormat="1" ht="25.5">
+      <c r="A2" s="16"/>
+      <c r="B2" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="D2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="11" t="s">
+      <c r="E2" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="11" t="s">
+      <c r="F2" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="12" t="s">
+      <c r="G2" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="5"/>
+      <c r="H2" s="14"/>
+      <c r="I2" s="10"/>
+      <c r="J2" s="7"/>
+      <c r="K2" s="10"/>
+      <c r="L2" s="7"/>
+      <c r="M2" s="10"/>
+      <c r="N2" s="7"/>
+      <c r="O2" s="10"/>
+      <c r="P2" s="7"/>
+      <c r="Q2" s="10"/>
+      <c r="R2" s="7"/>
+      <c r="S2" s="10"/>
+      <c r="T2" s="7"/>
+      <c r="U2" s="10"/>
+      <c r="V2" s="7"/>
+      <c r="W2" s="10"/>
+      <c r="X2" s="7"/>
+      <c r="Y2" s="10"/>
+      <c r="Z2" s="7"/>
+      <c r="AA2" s="10"/>
+      <c r="AB2" s="7"/>
+      <c r="AC2" s="10"/>
+      <c r="AD2" s="7"/>
+      <c r="AE2" s="10"/>
+      <c r="AF2" s="7"/>
+      <c r="AG2" s="10"/>
+      <c r="AH2" s="7"/>
+      <c r="AI2" s="10"/>
+      <c r="AJ2" s="7"/>
+      <c r="AK2" s="10"/>
+      <c r="AL2" s="7"/>
+      <c r="AM2" s="10"/>
+      <c r="AN2" s="7"/>
+      <c r="AO2" s="10"/>
+      <c r="AP2" s="7"/>
+      <c r="AQ2" s="10"/>
+      <c r="AR2" s="7"/>
+      <c r="AS2" s="10"/>
+      <c r="AT2" s="7"/>
+      <c r="AU2" s="10"/>
+      <c r="AV2" s="7"/>
+      <c r="AW2" s="10"/>
+      <c r="AX2" s="7"/>
+      <c r="AY2" s="10"/>
+      <c r="AZ2" s="7"/>
+      <c r="BA2" s="10"/>
+      <c r="BB2" s="7"/>
+      <c r="BC2" s="10"/>
+      <c r="BD2" s="7"/>
+      <c r="BE2" s="10"/>
+      <c r="BF2" s="7"/>
+      <c r="BG2" s="10"/>
+      <c r="BH2" s="7"/>
+      <c r="BI2" s="9"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="30">
+    <mergeCell ref="BG1:BH1"/>
+    <mergeCell ref="AW1:AX1"/>
+    <mergeCell ref="AY1:AZ1"/>
+    <mergeCell ref="BA1:BB1"/>
+    <mergeCell ref="BC1:BD1"/>
+    <mergeCell ref="BE1:BF1"/>
+    <mergeCell ref="AM1:AN1"/>
+    <mergeCell ref="AO1:AP1"/>
+    <mergeCell ref="AQ1:AR1"/>
+    <mergeCell ref="AS1:AT1"/>
+    <mergeCell ref="AU1:AV1"/>
+    <mergeCell ref="AC1:AD1"/>
+    <mergeCell ref="AE1:AF1"/>
+    <mergeCell ref="AG1:AH1"/>
+    <mergeCell ref="AI1:AJ1"/>
+    <mergeCell ref="AK1:AL1"/>
+    <mergeCell ref="U1:V1"/>
+    <mergeCell ref="W1:X1"/>
+    <mergeCell ref="Y1:Z1"/>
+    <mergeCell ref="AA1:AB1"/>
+    <mergeCell ref="K1:L1"/>
+    <mergeCell ref="M1:N1"/>
+    <mergeCell ref="O1:P1"/>
+    <mergeCell ref="Q1:R1"/>
+    <mergeCell ref="S1:T1"/>
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="E1:G1"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="H1:H2"/>
+    <mergeCell ref="I1:J1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="3" max="3" width="20.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>23</v>
+      </c>
+      <c r="C2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>35</v>
+      </c>
+      <c r="C3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>67</v>
+      </c>
+      <c r="C4">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Renamed experiment, reduced trials to 15 and implemented a mechanism to stop the engine when it is reasoning for more than 10 minutes
</commit_message>
<xml_diff>
--- a/madetools/core/src/main/resources/ExperimentSummary.xlsx
+++ b/madetools/core/src/main/resources/ExperimentSummary.xlsx
@@ -220,22 +220,22 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -550,7 +550,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="11" t="s">
         <v>16</v>
       </c>
       <c r="B1" s="2" t="s">
@@ -610,78 +610,78 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:61" s="2" customFormat="1">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="12"/>
+      <c r="C1" s="14"/>
       <c r="D1" s="13"/>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="12"/>
+      <c r="F1" s="14"/>
       <c r="G1" s="13"/>
-      <c r="H1" s="14" t="s">
+      <c r="H1" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="11"/>
+      <c r="I1" s="12"/>
       <c r="J1" s="13"/>
-      <c r="K1" s="11"/>
+      <c r="K1" s="12"/>
       <c r="L1" s="13"/>
-      <c r="M1" s="11"/>
+      <c r="M1" s="12"/>
       <c r="N1" s="13"/>
-      <c r="O1" s="11"/>
+      <c r="O1" s="12"/>
       <c r="P1" s="13"/>
-      <c r="Q1" s="11"/>
+      <c r="Q1" s="12"/>
       <c r="R1" s="13"/>
-      <c r="S1" s="11"/>
+      <c r="S1" s="12"/>
       <c r="T1" s="13"/>
-      <c r="U1" s="11"/>
+      <c r="U1" s="12"/>
       <c r="V1" s="13"/>
-      <c r="W1" s="11"/>
+      <c r="W1" s="12"/>
       <c r="X1" s="13"/>
-      <c r="Y1" s="11"/>
+      <c r="Y1" s="12"/>
       <c r="Z1" s="13"/>
-      <c r="AA1" s="11"/>
+      <c r="AA1" s="12"/>
       <c r="AB1" s="13"/>
-      <c r="AC1" s="11"/>
+      <c r="AC1" s="12"/>
       <c r="AD1" s="13"/>
-      <c r="AE1" s="11"/>
+      <c r="AE1" s="12"/>
       <c r="AF1" s="13"/>
-      <c r="AG1" s="11"/>
+      <c r="AG1" s="12"/>
       <c r="AH1" s="13"/>
-      <c r="AI1" s="11"/>
+      <c r="AI1" s="12"/>
       <c r="AJ1" s="13"/>
-      <c r="AK1" s="11"/>
+      <c r="AK1" s="12"/>
       <c r="AL1" s="13"/>
-      <c r="AM1" s="11"/>
+      <c r="AM1" s="12"/>
       <c r="AN1" s="13"/>
-      <c r="AO1" s="11"/>
+      <c r="AO1" s="12"/>
       <c r="AP1" s="13"/>
-      <c r="AQ1" s="11"/>
+      <c r="AQ1" s="12"/>
       <c r="AR1" s="13"/>
-      <c r="AS1" s="11"/>
+      <c r="AS1" s="12"/>
       <c r="AT1" s="13"/>
-      <c r="AU1" s="11"/>
+      <c r="AU1" s="12"/>
       <c r="AV1" s="13"/>
-      <c r="AW1" s="11"/>
+      <c r="AW1" s="12"/>
       <c r="AX1" s="13"/>
-      <c r="AY1" s="11"/>
+      <c r="AY1" s="12"/>
       <c r="AZ1" s="13"/>
-      <c r="BA1" s="11"/>
+      <c r="BA1" s="12"/>
       <c r="BB1" s="13"/>
-      <c r="BC1" s="11"/>
+      <c r="BC1" s="12"/>
       <c r="BD1" s="13"/>
-      <c r="BE1" s="11"/>
+      <c r="BE1" s="12"/>
       <c r="BF1" s="13"/>
-      <c r="BG1" s="11"/>
+      <c r="BG1" s="12"/>
       <c r="BH1" s="13"/>
       <c r="BI1" s="6"/>
     </row>
     <row r="2" spans="1:61" s="3" customFormat="1" ht="25.5">
-      <c r="A2" s="16"/>
+      <c r="A2" s="15"/>
       <c r="B2" s="10" t="s">
         <v>1</v>
       </c>
@@ -700,7 +700,7 @@
       <c r="G2" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="14"/>
+      <c r="H2" s="16"/>
       <c r="I2" s="10"/>
       <c r="J2" s="7"/>
       <c r="K2" s="10"/>
@@ -757,22 +757,11 @@
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="BG1:BH1"/>
-    <mergeCell ref="AW1:AX1"/>
-    <mergeCell ref="AY1:AZ1"/>
-    <mergeCell ref="BA1:BB1"/>
-    <mergeCell ref="BC1:BD1"/>
-    <mergeCell ref="BE1:BF1"/>
-    <mergeCell ref="AM1:AN1"/>
-    <mergeCell ref="AO1:AP1"/>
-    <mergeCell ref="AQ1:AR1"/>
-    <mergeCell ref="AS1:AT1"/>
-    <mergeCell ref="AU1:AV1"/>
-    <mergeCell ref="AC1:AD1"/>
-    <mergeCell ref="AE1:AF1"/>
-    <mergeCell ref="AG1:AH1"/>
-    <mergeCell ref="AI1:AJ1"/>
-    <mergeCell ref="AK1:AL1"/>
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="H1:H2"/>
+    <mergeCell ref="I1:J1"/>
     <mergeCell ref="U1:V1"/>
     <mergeCell ref="W1:X1"/>
     <mergeCell ref="Y1:Z1"/>
@@ -782,11 +771,22 @@
     <mergeCell ref="O1:P1"/>
     <mergeCell ref="Q1:R1"/>
     <mergeCell ref="S1:T1"/>
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="E1:G1"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="H1:H2"/>
-    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="AC1:AD1"/>
+    <mergeCell ref="AE1:AF1"/>
+    <mergeCell ref="AG1:AH1"/>
+    <mergeCell ref="AI1:AJ1"/>
+    <mergeCell ref="AK1:AL1"/>
+    <mergeCell ref="AM1:AN1"/>
+    <mergeCell ref="AO1:AP1"/>
+    <mergeCell ref="AQ1:AR1"/>
+    <mergeCell ref="AS1:AT1"/>
+    <mergeCell ref="AU1:AV1"/>
+    <mergeCell ref="BG1:BH1"/>
+    <mergeCell ref="AW1:AX1"/>
+    <mergeCell ref="AY1:AZ1"/>
+    <mergeCell ref="BA1:BB1"/>
+    <mergeCell ref="BC1:BD1"/>
+    <mergeCell ref="BE1:BF1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -795,10 +795,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -817,39 +817,6 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
-      <c r="A2">
-        <v>0</v>
-      </c>
-      <c r="B2">
-        <v>23</v>
-      </c>
-      <c r="C2">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3">
-        <v>35</v>
-      </c>
-      <c r="C3">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4">
-        <v>2</v>
-      </c>
-      <c r="B4">
-        <v>67</v>
-      </c>
-      <c r="C4">
-        <v>15</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added a new experiment where we give more fitness for ocuurrences of new tropes than to ocurrences of previously found tropes. Implemented parallelism of simulations. Changed maximum wait time to 5 minutes. Added time of execution.
</commit_message>
<xml_diff>
--- a/madetools/core/src/main/resources/ExperimentSummary.xlsx
+++ b/madetools/core/src/main/resources/ExperimentSummary.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="19">
   <si>
     <t>Iteration</t>
   </si>
@@ -70,6 +70,9 @@
   </si>
   <si>
     <t>1.0</t>
+  </si>
+  <si>
+    <t>Execution time (ms)</t>
   </si>
 </sst>
 </file>
@@ -188,7 +191,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -226,16 +229,19 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -536,7 +542,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
   <cols>
@@ -594,199 +602,204 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:BI2"/>
+  <dimension ref="A1:BJ2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" style="8" customWidth="1"/>
-    <col min="2" max="7" width="11.42578125" style="8"/>
-    <col min="8" max="8" width="55.140625" style="8" customWidth="1"/>
-    <col min="9" max="61" width="11.42578125" style="8"/>
-    <col min="62" max="16384" width="11.42578125" style="1"/>
+    <col min="1" max="2" width="11.42578125" style="8" customWidth="1"/>
+    <col min="3" max="8" width="11.42578125" style="8"/>
+    <col min="9" max="9" width="55.140625" style="8" customWidth="1"/>
+    <col min="10" max="62" width="11.42578125" style="8"/>
+    <col min="63" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:61" s="2" customFormat="1">
-      <c r="A1" s="15" t="s">
+    <row r="1" spans="1:62" s="2" customFormat="1">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="14"/>
       <c r="D1" s="13"/>
-      <c r="E1" s="12" t="s">
+      <c r="E1" s="14"/>
+      <c r="F1" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="14"/>
       <c r="G1" s="13"/>
-      <c r="H1" s="16" t="s">
+      <c r="H1" s="14"/>
+      <c r="I1" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="12"/>
-      <c r="J1" s="13"/>
-      <c r="K1" s="12"/>
-      <c r="L1" s="13"/>
-      <c r="M1" s="12"/>
-      <c r="N1" s="13"/>
-      <c r="O1" s="12"/>
-      <c r="P1" s="13"/>
-      <c r="Q1" s="12"/>
-      <c r="R1" s="13"/>
-      <c r="S1" s="12"/>
-      <c r="T1" s="13"/>
-      <c r="U1" s="12"/>
-      <c r="V1" s="13"/>
-      <c r="W1" s="12"/>
-      <c r="X1" s="13"/>
-      <c r="Y1" s="12"/>
-      <c r="Z1" s="13"/>
-      <c r="AA1" s="12"/>
-      <c r="AB1" s="13"/>
-      <c r="AC1" s="12"/>
-      <c r="AD1" s="13"/>
-      <c r="AE1" s="12"/>
-      <c r="AF1" s="13"/>
-      <c r="AG1" s="12"/>
-      <c r="AH1" s="13"/>
-      <c r="AI1" s="12"/>
-      <c r="AJ1" s="13"/>
-      <c r="AK1" s="12"/>
-      <c r="AL1" s="13"/>
-      <c r="AM1" s="12"/>
-      <c r="AN1" s="13"/>
-      <c r="AO1" s="12"/>
-      <c r="AP1" s="13"/>
-      <c r="AQ1" s="12"/>
-      <c r="AR1" s="13"/>
-      <c r="AS1" s="12"/>
-      <c r="AT1" s="13"/>
-      <c r="AU1" s="12"/>
-      <c r="AV1" s="13"/>
-      <c r="AW1" s="12"/>
-      <c r="AX1" s="13"/>
-      <c r="AY1" s="12"/>
-      <c r="AZ1" s="13"/>
-      <c r="BA1" s="12"/>
-      <c r="BB1" s="13"/>
-      <c r="BC1" s="12"/>
-      <c r="BD1" s="13"/>
-      <c r="BE1" s="12"/>
-      <c r="BF1" s="13"/>
-      <c r="BG1" s="12"/>
-      <c r="BH1" s="13"/>
-      <c r="BI1" s="6"/>
+      <c r="J1" s="12"/>
+      <c r="K1" s="14"/>
+      <c r="L1" s="12"/>
+      <c r="M1" s="14"/>
+      <c r="N1" s="12"/>
+      <c r="O1" s="14"/>
+      <c r="P1" s="12"/>
+      <c r="Q1" s="14"/>
+      <c r="R1" s="12"/>
+      <c r="S1" s="14"/>
+      <c r="T1" s="12"/>
+      <c r="U1" s="14"/>
+      <c r="V1" s="12"/>
+      <c r="W1" s="14"/>
+      <c r="X1" s="12"/>
+      <c r="Y1" s="14"/>
+      <c r="Z1" s="12"/>
+      <c r="AA1" s="14"/>
+      <c r="AB1" s="12"/>
+      <c r="AC1" s="14"/>
+      <c r="AD1" s="12"/>
+      <c r="AE1" s="14"/>
+      <c r="AF1" s="12"/>
+      <c r="AG1" s="14"/>
+      <c r="AH1" s="12"/>
+      <c r="AI1" s="14"/>
+      <c r="AJ1" s="12"/>
+      <c r="AK1" s="14"/>
+      <c r="AL1" s="12"/>
+      <c r="AM1" s="14"/>
+      <c r="AN1" s="12"/>
+      <c r="AO1" s="14"/>
+      <c r="AP1" s="12"/>
+      <c r="AQ1" s="14"/>
+      <c r="AR1" s="12"/>
+      <c r="AS1" s="14"/>
+      <c r="AT1" s="12"/>
+      <c r="AU1" s="14"/>
+      <c r="AV1" s="12"/>
+      <c r="AW1" s="14"/>
+      <c r="AX1" s="12"/>
+      <c r="AY1" s="14"/>
+      <c r="AZ1" s="12"/>
+      <c r="BA1" s="14"/>
+      <c r="BB1" s="12"/>
+      <c r="BC1" s="14"/>
+      <c r="BD1" s="12"/>
+      <c r="BE1" s="14"/>
+      <c r="BF1" s="12"/>
+      <c r="BG1" s="14"/>
+      <c r="BH1" s="12"/>
+      <c r="BI1" s="14"/>
+      <c r="BJ1" s="6"/>
     </row>
-    <row r="2" spans="1:61" s="3" customFormat="1" ht="25.5">
+    <row r="2" spans="1:62" s="3" customFormat="1" ht="25.5">
       <c r="A2" s="15"/>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="16"/>
+      <c r="C2" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="D2" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="E2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="F2" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="G2" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="H2" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="16"/>
-      <c r="I2" s="10"/>
-      <c r="J2" s="7"/>
-      <c r="K2" s="10"/>
-      <c r="L2" s="7"/>
-      <c r="M2" s="10"/>
-      <c r="N2" s="7"/>
-      <c r="O2" s="10"/>
-      <c r="P2" s="7"/>
-      <c r="Q2" s="10"/>
-      <c r="R2" s="7"/>
-      <c r="S2" s="10"/>
-      <c r="T2" s="7"/>
-      <c r="U2" s="10"/>
-      <c r="V2" s="7"/>
-      <c r="W2" s="10"/>
-      <c r="X2" s="7"/>
-      <c r="Y2" s="10"/>
-      <c r="Z2" s="7"/>
-      <c r="AA2" s="10"/>
-      <c r="AB2" s="7"/>
-      <c r="AC2" s="10"/>
-      <c r="AD2" s="7"/>
-      <c r="AE2" s="10"/>
-      <c r="AF2" s="7"/>
-      <c r="AG2" s="10"/>
-      <c r="AH2" s="7"/>
-      <c r="AI2" s="10"/>
-      <c r="AJ2" s="7"/>
-      <c r="AK2" s="10"/>
-      <c r="AL2" s="7"/>
-      <c r="AM2" s="10"/>
-      <c r="AN2" s="7"/>
-      <c r="AO2" s="10"/>
-      <c r="AP2" s="7"/>
-      <c r="AQ2" s="10"/>
-      <c r="AR2" s="7"/>
-      <c r="AS2" s="10"/>
-      <c r="AT2" s="7"/>
-      <c r="AU2" s="10"/>
-      <c r="AV2" s="7"/>
-      <c r="AW2" s="10"/>
-      <c r="AX2" s="7"/>
-      <c r="AY2" s="10"/>
-      <c r="AZ2" s="7"/>
-      <c r="BA2" s="10"/>
-      <c r="BB2" s="7"/>
-      <c r="BC2" s="10"/>
-      <c r="BD2" s="7"/>
-      <c r="BE2" s="10"/>
-      <c r="BF2" s="7"/>
-      <c r="BG2" s="10"/>
-      <c r="BH2" s="7"/>
-      <c r="BI2" s="9"/>
+      <c r="I2" s="16"/>
+      <c r="J2" s="10"/>
+      <c r="K2" s="7"/>
+      <c r="L2" s="10"/>
+      <c r="M2" s="7"/>
+      <c r="N2" s="10"/>
+      <c r="O2" s="7"/>
+      <c r="P2" s="10"/>
+      <c r="Q2" s="7"/>
+      <c r="R2" s="10"/>
+      <c r="S2" s="7"/>
+      <c r="T2" s="10"/>
+      <c r="U2" s="7"/>
+      <c r="V2" s="10"/>
+      <c r="W2" s="7"/>
+      <c r="X2" s="10"/>
+      <c r="Y2" s="7"/>
+      <c r="Z2" s="10"/>
+      <c r="AA2" s="7"/>
+      <c r="AB2" s="10"/>
+      <c r="AC2" s="7"/>
+      <c r="AD2" s="10"/>
+      <c r="AE2" s="7"/>
+      <c r="AF2" s="10"/>
+      <c r="AG2" s="7"/>
+      <c r="AH2" s="10"/>
+      <c r="AI2" s="7"/>
+      <c r="AJ2" s="10"/>
+      <c r="AK2" s="7"/>
+      <c r="AL2" s="10"/>
+      <c r="AM2" s="7"/>
+      <c r="AN2" s="10"/>
+      <c r="AO2" s="7"/>
+      <c r="AP2" s="10"/>
+      <c r="AQ2" s="7"/>
+      <c r="AR2" s="10"/>
+      <c r="AS2" s="7"/>
+      <c r="AT2" s="10"/>
+      <c r="AU2" s="7"/>
+      <c r="AV2" s="10"/>
+      <c r="AW2" s="7"/>
+      <c r="AX2" s="10"/>
+      <c r="AY2" s="7"/>
+      <c r="AZ2" s="10"/>
+      <c r="BA2" s="7"/>
+      <c r="BB2" s="10"/>
+      <c r="BC2" s="7"/>
+      <c r="BD2" s="10"/>
+      <c r="BE2" s="7"/>
+      <c r="BF2" s="10"/>
+      <c r="BG2" s="7"/>
+      <c r="BH2" s="10"/>
+      <c r="BI2" s="7"/>
+      <c r="BJ2" s="9"/>
     </row>
   </sheetData>
-  <mergeCells count="30">
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="E1:G1"/>
+  <mergeCells count="31">
+    <mergeCell ref="BH1:BI1"/>
+    <mergeCell ref="AX1:AY1"/>
+    <mergeCell ref="AZ1:BA1"/>
+    <mergeCell ref="BB1:BC1"/>
+    <mergeCell ref="BD1:BE1"/>
+    <mergeCell ref="BF1:BG1"/>
+    <mergeCell ref="AN1:AO1"/>
+    <mergeCell ref="AP1:AQ1"/>
+    <mergeCell ref="AR1:AS1"/>
+    <mergeCell ref="AT1:AU1"/>
+    <mergeCell ref="AV1:AW1"/>
+    <mergeCell ref="AD1:AE1"/>
+    <mergeCell ref="AF1:AG1"/>
+    <mergeCell ref="AH1:AI1"/>
+    <mergeCell ref="AJ1:AK1"/>
+    <mergeCell ref="AL1:AM1"/>
+    <mergeCell ref="V1:W1"/>
+    <mergeCell ref="X1:Y1"/>
+    <mergeCell ref="Z1:AA1"/>
+    <mergeCell ref="AB1:AC1"/>
+    <mergeCell ref="L1:M1"/>
+    <mergeCell ref="N1:O1"/>
+    <mergeCell ref="P1:Q1"/>
+    <mergeCell ref="R1:S1"/>
+    <mergeCell ref="T1:U1"/>
+    <mergeCell ref="C1:E1"/>
+    <mergeCell ref="F1:H1"/>
     <mergeCell ref="A1:A2"/>
-    <mergeCell ref="H1:H2"/>
-    <mergeCell ref="I1:J1"/>
-    <mergeCell ref="U1:V1"/>
-    <mergeCell ref="W1:X1"/>
-    <mergeCell ref="Y1:Z1"/>
-    <mergeCell ref="AA1:AB1"/>
-    <mergeCell ref="K1:L1"/>
-    <mergeCell ref="M1:N1"/>
-    <mergeCell ref="O1:P1"/>
-    <mergeCell ref="Q1:R1"/>
-    <mergeCell ref="S1:T1"/>
-    <mergeCell ref="AC1:AD1"/>
-    <mergeCell ref="AE1:AF1"/>
-    <mergeCell ref="AG1:AH1"/>
-    <mergeCell ref="AI1:AJ1"/>
-    <mergeCell ref="AK1:AL1"/>
-    <mergeCell ref="AM1:AN1"/>
-    <mergeCell ref="AO1:AP1"/>
-    <mergeCell ref="AQ1:AR1"/>
-    <mergeCell ref="AS1:AT1"/>
-    <mergeCell ref="AU1:AV1"/>
-    <mergeCell ref="BG1:BH1"/>
-    <mergeCell ref="AW1:AX1"/>
-    <mergeCell ref="AY1:AZ1"/>
-    <mergeCell ref="BA1:BB1"/>
-    <mergeCell ref="BC1:BD1"/>
-    <mergeCell ref="BE1:BF1"/>
+    <mergeCell ref="I1:I2"/>
+    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="B1:B2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>